<commit_message>
Moved product backlog into sperate excel file and added formatting to Project Plan document
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlogs.xlsx
+++ b/Documentation/Sprint Backlogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Functional Requirement</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>2 days</t>
+  </si>
+  <si>
+    <t>Add uniform formatting to documents</t>
+  </si>
+  <si>
+    <t>1 hour</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -135,18 +141,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -478,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:F10"/>
+  <dimension ref="C4:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +602,20 @@
       </c>
       <c r="F10" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>